<commit_message>
Add cell coloring feature
</commit_message>
<xml_diff>
--- a/sample_addresses.xlsx
+++ b/sample_addresses.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.222\pi\ram\geo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D739980-E299-41F8-BD6A-D468798C1292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80625C2-92EC-447E-AFF0-B3012AB5CD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{1497F488-97BA-4FD4-99D3-9DFC8FF2E4FA}"/>
+    <workbookView xWindow="2760" yWindow="3192" windowWidth="17280" windowHeight="8964" xr2:uid="{1497F488-97BA-4FD4-99D3-9DFC8FF2E4FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Addresses" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
-  <si>
-    <t>Postal code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>City</t>
   </si>
@@ -60,9 +57,6 @@
     <t>555-12345</t>
   </si>
   <si>
-    <t>Birth Date</t>
-  </si>
-  <si>
     <t>Beach House</t>
   </si>
   <si>
@@ -142,14 +136,85 @@
   </si>
   <si>
     <t>info@disney.com</t>
+  </si>
+  <si>
+    <t>AVENUE DU 8 MAI 1945</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Brant Home</t>
+  </si>
+  <si>
+    <t>Brantome</t>
+  </si>
+  <si>
+    <t>55.44.33.22.11</t>
+  </si>
+  <si>
+    <t>contact@brant.com</t>
+  </si>
+  <si>
+    <t>info@rozana.pl</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>10005</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>90254</t>
+  </si>
+  <si>
+    <t>32830</t>
+  </si>
+  <si>
+    <t>24310</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Bad Street</t>
+  </si>
+  <si>
+    <t>Wrong City</t>
+  </si>
+  <si>
+    <t>99999</t>
+  </si>
+  <si>
+    <t>XY</t>
+  </si>
+  <si>
+    <t>info@bad.er</t>
+  </si>
+  <si>
+    <t>00.12.34.56</t>
+  </si>
+  <si>
+    <t>Bad, so bad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,13 +242,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +573,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4366F61-AE72-4F44-AFC5-BA3F302AEF78}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -506,152 +581,201 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2">
-        <v>10005</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="C3">
-        <v>8000</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>90254</v>
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
+        <v>52</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5">
-        <v>32830</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>